<commit_message>
Added OmegaBoardPosition(fen), toFENString and toBoardString.
Also minor fixes
</commit_message>
<xml_diff>
--- a/fields.xlsx
+++ b/fields.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fkopp/Dropbox/Private/Projekte/Java/_GITHUB/Chessly/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frank\Dropbox\Private\Projekte\Java\_GITHUB\Chessly\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16380" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16380" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="136">
   <si>
     <t>a1</t>
   </si>
@@ -408,6 +409,30 @@
   </si>
   <si>
     <t>p8</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
   </si>
 </sst>
 </file>
@@ -430,15 +455,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -446,22 +477,173 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -732,31 +914,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView zoomScale="180" workbookViewId="0">
+      <selection sqref="A1:P16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -813,7 +995,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -871,12 +1053,12 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:F16" si="0">B2+1</f>
+        <f t="shared" ref="B3:B16" si="0">B2+1</f>
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -929,7 +1111,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -987,7 +1169,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -1045,7 +1227,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -1103,7 +1285,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -1161,7 +1343,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -1219,7 +1401,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>64</v>
       </c>
@@ -1277,7 +1459,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>65</v>
       </c>
@@ -1335,7 +1517,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>66</v>
       </c>
@@ -1393,7 +1575,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>67</v>
       </c>
@@ -1451,7 +1633,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>68</v>
       </c>
@@ -1509,7 +1691,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>69</v>
       </c>
@@ -1567,7 +1749,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>70</v>
       </c>
@@ -1625,7 +1807,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>71</v>
       </c>
@@ -1687,4 +1869,601 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="1.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="17" width="3.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>8</v>
+      </c>
+      <c r="B2" s="5">
+        <f t="shared" ref="B2:B7" si="0">B3+16</f>
+        <v>112</v>
+      </c>
+      <c r="C2" s="6">
+        <f t="shared" ref="C2:C7" si="1">C3+16</f>
+        <v>113</v>
+      </c>
+      <c r="D2" s="6">
+        <f t="shared" ref="D2:D7" si="2">D3+16</f>
+        <v>114</v>
+      </c>
+      <c r="E2" s="6">
+        <f t="shared" ref="E2:E7" si="3">E3+16</f>
+        <v>115</v>
+      </c>
+      <c r="F2" s="6">
+        <f t="shared" ref="F2:F7" si="4">F3+16</f>
+        <v>116</v>
+      </c>
+      <c r="G2" s="6">
+        <f t="shared" ref="G2:G7" si="5">G3+16</f>
+        <v>117</v>
+      </c>
+      <c r="H2" s="6">
+        <f t="shared" ref="H2:H7" si="6">H3+16</f>
+        <v>118</v>
+      </c>
+      <c r="I2" s="7">
+        <f t="shared" ref="I2:I7" si="7">I3+16</f>
+        <v>119</v>
+      </c>
+      <c r="J2">
+        <f t="shared" ref="J2:J7" si="8">J3+16</f>
+        <v>120</v>
+      </c>
+      <c r="K2">
+        <f t="shared" ref="K2:K7" si="9">K3+16</f>
+        <v>121</v>
+      </c>
+      <c r="L2">
+        <f t="shared" ref="L2:L7" si="10">L3+16</f>
+        <v>122</v>
+      </c>
+      <c r="M2">
+        <f t="shared" ref="M2:M7" si="11">M3+16</f>
+        <v>123</v>
+      </c>
+      <c r="N2">
+        <f t="shared" ref="N2:N7" si="12">N3+16</f>
+        <v>124</v>
+      </c>
+      <c r="O2">
+        <f t="shared" ref="O2:O7" si="13">O3+16</f>
+        <v>125</v>
+      </c>
+      <c r="P2">
+        <f t="shared" ref="P2:P7" si="14">P3+16</f>
+        <v>126</v>
+      </c>
+      <c r="Q2">
+        <f t="shared" ref="Q2:Q7" si="15">Q3+16</f>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>7</v>
+      </c>
+      <c r="B3" s="8">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="C3" s="4">
+        <f t="shared" si="1"/>
+        <v>97</v>
+      </c>
+      <c r="D3" s="4">
+        <f t="shared" si="2"/>
+        <v>98</v>
+      </c>
+      <c r="E3" s="4">
+        <f t="shared" si="3"/>
+        <v>99</v>
+      </c>
+      <c r="F3" s="4">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+      <c r="G3" s="4">
+        <f t="shared" si="5"/>
+        <v>101</v>
+      </c>
+      <c r="H3" s="4">
+        <f t="shared" si="6"/>
+        <v>102</v>
+      </c>
+      <c r="I3" s="9">
+        <f t="shared" si="7"/>
+        <v>103</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="8"/>
+        <v>104</v>
+      </c>
+      <c r="K3">
+        <f t="shared" si="9"/>
+        <v>105</v>
+      </c>
+      <c r="L3">
+        <f t="shared" si="10"/>
+        <v>106</v>
+      </c>
+      <c r="M3">
+        <f t="shared" si="11"/>
+        <v>107</v>
+      </c>
+      <c r="N3">
+        <f t="shared" si="12"/>
+        <v>108</v>
+      </c>
+      <c r="O3">
+        <f t="shared" si="13"/>
+        <v>109</v>
+      </c>
+      <c r="P3">
+        <f t="shared" si="14"/>
+        <v>110</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" si="15"/>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>6</v>
+      </c>
+      <c r="B4" s="8">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="C4" s="4">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+      <c r="D4" s="4">
+        <f t="shared" si="2"/>
+        <v>82</v>
+      </c>
+      <c r="E4" s="4">
+        <f t="shared" si="3"/>
+        <v>83</v>
+      </c>
+      <c r="F4" s="4">
+        <f t="shared" si="4"/>
+        <v>84</v>
+      </c>
+      <c r="G4" s="4">
+        <f t="shared" si="5"/>
+        <v>85</v>
+      </c>
+      <c r="H4" s="4">
+        <f t="shared" si="6"/>
+        <v>86</v>
+      </c>
+      <c r="I4" s="9">
+        <f t="shared" si="7"/>
+        <v>87</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="8"/>
+        <v>88</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="9"/>
+        <v>89</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="10"/>
+        <v>90</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="11"/>
+        <v>91</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="12"/>
+        <v>92</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="13"/>
+        <v>93</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="14"/>
+        <v>94</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="15"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>5</v>
+      </c>
+      <c r="B5" s="8">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="C5" s="4">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="D5" s="4">
+        <f t="shared" si="2"/>
+        <v>66</v>
+      </c>
+      <c r="E5" s="4">
+        <f t="shared" si="3"/>
+        <v>67</v>
+      </c>
+      <c r="F5" s="4">
+        <f t="shared" si="4"/>
+        <v>68</v>
+      </c>
+      <c r="G5" s="4">
+        <f t="shared" si="5"/>
+        <v>69</v>
+      </c>
+      <c r="H5" s="4">
+        <f t="shared" si="6"/>
+        <v>70</v>
+      </c>
+      <c r="I5" s="9">
+        <f t="shared" si="7"/>
+        <v>71</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="8"/>
+        <v>72</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="9"/>
+        <v>73</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="10"/>
+        <v>74</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="11"/>
+        <v>75</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="12"/>
+        <v>76</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="13"/>
+        <v>77</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="14"/>
+        <v>78</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="15"/>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="8">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="C6" s="4">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="D6" s="4">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="E6" s="4">
+        <f t="shared" si="3"/>
+        <v>51</v>
+      </c>
+      <c r="F6" s="4">
+        <f t="shared" si="4"/>
+        <v>52</v>
+      </c>
+      <c r="G6" s="4">
+        <f t="shared" si="5"/>
+        <v>53</v>
+      </c>
+      <c r="H6" s="4">
+        <f t="shared" si="6"/>
+        <v>54</v>
+      </c>
+      <c r="I6" s="9">
+        <f t="shared" si="7"/>
+        <v>55</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="8"/>
+        <v>56</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="9"/>
+        <v>57</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="10"/>
+        <v>58</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="11"/>
+        <v>59</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="12"/>
+        <v>60</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="13"/>
+        <v>61</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="14"/>
+        <v>62</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="15"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>3</v>
+      </c>
+      <c r="B7" s="8">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="C7" s="4">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="D7" s="4">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="E7" s="4">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="F7" s="4">
+        <f t="shared" si="4"/>
+        <v>36</v>
+      </c>
+      <c r="G7" s="4">
+        <f t="shared" si="5"/>
+        <v>37</v>
+      </c>
+      <c r="H7" s="4">
+        <f t="shared" si="6"/>
+        <v>38</v>
+      </c>
+      <c r="I7" s="9">
+        <f t="shared" si="7"/>
+        <v>39</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="8"/>
+        <v>40</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="9"/>
+        <v>41</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="10"/>
+        <v>42</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="11"/>
+        <v>43</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="12"/>
+        <v>44</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="14"/>
+        <v>46</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="15"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>2</v>
+      </c>
+      <c r="B8" s="8">
+        <f>B9+16</f>
+        <v>16</v>
+      </c>
+      <c r="C8" s="4">
+        <f t="shared" ref="C8:Q8" si="16">C9+16</f>
+        <v>17</v>
+      </c>
+      <c r="D8" s="4">
+        <f t="shared" si="16"/>
+        <v>18</v>
+      </c>
+      <c r="E8" s="4">
+        <f t="shared" si="16"/>
+        <v>19</v>
+      </c>
+      <c r="F8" s="4">
+        <f t="shared" si="16"/>
+        <v>20</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" si="16"/>
+        <v>21</v>
+      </c>
+      <c r="H8" s="4">
+        <f t="shared" si="16"/>
+        <v>22</v>
+      </c>
+      <c r="I8" s="9">
+        <f t="shared" si="16"/>
+        <v>23</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="16"/>
+        <v>24</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="16"/>
+        <v>25</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="16"/>
+        <v>26</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="16"/>
+        <v>27</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="16"/>
+        <v>28</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="16"/>
+        <v>29</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="16"/>
+        <v>30</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="16"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>1</v>
+      </c>
+      <c r="B9" s="10">
+        <v>0</v>
+      </c>
+      <c r="C9" s="11">
+        <f>B9+1</f>
+        <v>1</v>
+      </c>
+      <c r="D9" s="11">
+        <f t="shared" ref="D9:Q9" si="17">C9+1</f>
+        <v>2</v>
+      </c>
+      <c r="E9" s="11">
+        <f t="shared" si="17"/>
+        <v>3</v>
+      </c>
+      <c r="F9" s="11">
+        <f t="shared" si="17"/>
+        <v>4</v>
+      </c>
+      <c r="G9" s="11">
+        <f t="shared" si="17"/>
+        <v>5</v>
+      </c>
+      <c r="H9" s="11">
+        <f t="shared" si="17"/>
+        <v>6</v>
+      </c>
+      <c r="I9" s="12">
+        <f t="shared" si="17"/>
+        <v>7</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="17"/>
+        <v>9</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="17"/>
+        <v>10</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="17"/>
+        <v>11</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="17"/>
+        <v>12</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="17"/>
+        <v>13</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="17"/>
+        <v>14</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="17"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added OmegaMove convert to GameMove and back
</commit_message>
<xml_diff>
--- a/fields.xlsx
+++ b/fields.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="146">
   <si>
     <t>a1</t>
   </si>
@@ -455,6 +455,15 @@
   </si>
   <si>
     <t>Movetype</t>
+  </si>
+  <si>
+    <t>Promotion</t>
+  </si>
+  <si>
+    <t>Castling</t>
+  </si>
+  <si>
+    <t>ff</t>
   </si>
 </sst>
 </file>
@@ -2501,17 +2510,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ6"/>
+  <dimension ref="A1:AJ9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="32" width="2.875" customWidth="1"/>
     <col min="34" max="34" width="5.375" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="7.625" customWidth="1"/>
+    <col min="35" max="35" width="9.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.25">
@@ -2746,6 +2755,9 @@
       </c>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>1</v>
+      </c>
       <c r="H6">
         <v>1</v>
       </c>
@@ -2756,18 +2768,81 @@
         <v>1</v>
       </c>
       <c r="AG6" t="s">
-        <v>142</v>
-      </c>
-      <c r="AH6">
-        <v>7</v>
+        <v>143</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>133</v>
       </c>
       <c r="AI6" t="str">
         <f>HEX2BIN(AH6)</f>
-        <v>111</v>
+        <v>1111</v>
       </c>
       <c r="AJ6">
         <f>HEX2DEC(AH6)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>142</v>
+      </c>
+      <c r="AH7">
         <v>7</v>
+      </c>
+      <c r="AI7" t="str">
+        <f>HEX2BIN(AH7)</f>
+        <v>111</v>
+      </c>
+      <c r="AJ7">
+        <f>HEX2DEC(AH7)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>144</v>
+      </c>
+      <c r="AH8">
+        <v>7</v>
+      </c>
+      <c r="AI8" t="str">
+        <f>HEX2BIN(AH8)</f>
+        <v>111</v>
+      </c>
+      <c r="AJ8">
+        <f>HEX2DEC(AH8)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AH9" t="s">
+        <v>145</v>
+      </c>
+      <c r="AI9" t="str">
+        <f>HEX2BIN(AH9)</f>
+        <v>11111111</v>
+      </c>
+      <c r="AJ9">
+        <f>HEX2DEC(AH9)</f>
+        <v>255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>